<commit_message>
Updated figures of aquaucltuer sustainability indicators (to use in the paper and, possibly, on the webiste).
Also, added trends of PRR idnex.
The table on neigbour municipalities - no chagnes, jsut opened and closed.
</commit_message>
<xml_diff>
--- a/prep/food_provision/Mariculture/data/neighbour_mcp_edited.xlsx
+++ b/prep/food_provision/Mariculture/data/neighbour_mcp_edited.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/nor-prep/prep/food_provision/mariculture/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{368CA61E-A38C-DE49-B698-B0DD639A8C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6F28AC-F940-2948-A912-BE97B2735D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="540" windowWidth="33140" windowHeight="26880" xr2:uid="{4EA9365E-3C65-694A-A48F-411CE11AD962}"/>
+    <workbookView xWindow="14180" yWindow="14320" windowWidth="30200" windowHeight="26700" xr2:uid="{4EA9365E-3C65-694A-A48F-411CE11AD962}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -772,7 +772,7 @@
   <dimension ref="A1:AA82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>